<commit_message>
Fixed missing values in the data
</commit_message>
<xml_diff>
--- a/Data/RAW_Excel/Receiver deployment sheet_Sept 2022_RAW.xlsx
+++ b/Data/RAW_Excel/Receiver deployment sheet_Sept 2022_RAW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Palau\Research\Coastal Fisheries\Natalie Tagging\2022 Bohar tagging\Bohar_2022_2023\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Palau\Research\Coastal Fisheries\Natalie Tagging\2022 Bohar tagging\Bohar_2022_2023\Data\RAW_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6F69C4-0D1C-4DEC-80E4-5E6D0D5A069B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1013323C-DFC2-48C2-B2B2-3A999A07366D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13016,13 +13016,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DE0EA2-0F9A-4358-8666-6AAC71698651}">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G20" sqref="G19:G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.27734375" style="15" customWidth="1"/>
     <col min="3" max="3" width="16.0546875" style="15" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="15"/>

</xml_diff>